<commit_message>
Big changes to positioning as well as some additional .py code. ADdition of NON-COVID player stats
</commit_message>
<xml_diff>
--- a/COVID NFLStats/CB/CB_aggregate.xlsx
+++ b/COVID NFLStats/CB/CB_aggregate.xlsx
@@ -495,55 +495,55 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Stephon Gilmore</t>
+          <t>Charvarius Ward</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>2019-2021</t>
+          <t>Group1</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>8.33333333333333</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>35.3333333333333</v>
+        <v>64</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>29.6666666666667</v>
+        <v>47.33333333333334</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>5.66666666666667</v>
+        <v>16.66666666666667</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Stephon Gilmore</t>
+          <t>Charvarius Ward</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>2022-2024</t>
+          <t>Group2</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>11</v>
+        <v>13.66666666666667</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>63.3333333333333</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>14.3333333333333</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Stephon Gilmore</t>
+          <t>Charvarius Ward</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>2.66666666666667</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>19.3333333333333</v>
+        <v>3.666666666666664</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>8.66666666666667</v>
+        <v>3.333333333333332</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Denzel Ward</t>
+          <t>D.J. Reed</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -576,22 +576,22 @@
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>13</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>44.3333333333333</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>36.6666666666667</v>
+        <v>39.66666666666666</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>7.66666666666667</v>
+        <v>11.33333333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Denzel Ward</t>
+          <t>D.J. Reed</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -600,22 +600,22 @@
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>15</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>45.3333333333333</v>
+        <v>73.33333333333333</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>37.6666666666667</v>
+        <v>59</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>7.66666666666667</v>
+        <v>14.33333333333333</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Denzel Ward</t>
+          <t>D.J. Reed</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -624,22 +624,22 @@
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>2</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1</v>
+        <v>22.33333333333333</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>1</v>
+        <v>19.33333333333334</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Isaac Yiadom</t>
+          <t>Denzel Ward</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -648,22 +648,22 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>33</v>
+        <v>44.33333333333334</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>23.3333333333333</v>
+        <v>36.66666666666666</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>9.66666666666667</v>
+        <v>7.666666666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Isaac Yiadom</t>
+          <t>Denzel Ward</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>6.66666666666667</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>28.1111111111111</v>
+        <v>45.33333333333334</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>21.2222222222222</v>
+        <v>37.66666666666666</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>6.88888888888889</v>
+        <v>7.666666666666667</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Isaac Yiadom</t>
+          <t>Denzel Ward</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>3.66666666666667</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>-4.88888888888889</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>-2.11111111111111</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-2.77777777777778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Charvarius Ward</t>
+          <t>Isaac Yiadom</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -720,22 +720,22 @@
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>8.66666666666667</v>
+        <v>3</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>47.3333333333333</v>
+        <v>23.33333333333333</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>16.6666666666667</v>
+        <v>9.666666666666666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Charvarius Ward</t>
+          <t>Isaac Yiadom</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -744,22 +744,22 @@
         </is>
       </c>
       <c r="C12" s="3" t="n">
-        <v>13.6666666666667</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>71</v>
+        <v>28.11111111111111</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>51</v>
+        <v>21.22222222222222</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>20</v>
+        <v>6.888888888888888</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Charvarius Ward</t>
+          <t>Isaac Yiadom</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -768,16 +768,16 @@
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>5</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>7</v>
+        <v>-4.888888888888886</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>3.66666666666666</v>
+        <v>-2.111111111111107</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>3.33333333333333</v>
+        <v>-2.777777777777778</v>
       </c>
     </row>
     <row r="14">
@@ -792,16 +792,16 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.333333333333333</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>15.6666666666667</v>
+        <v>15.66666666666667</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>13</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>2.66666666666667</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -822,10 +822,10 @@
         <v>18</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>9.33333333333333</v>
+        <v>9.333333333333334</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>8.66666666666667</v>
+        <v>8.666666666666666</v>
       </c>
     </row>
     <row r="16">
@@ -840,13 +840,13 @@
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>-0.333333333333333</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2.33333333333333</v>
+        <v>2.333333333333334</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-3.66666666666667</v>
+        <v>-3.666666666666666</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>6</v>
@@ -855,7 +855,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Mike Ford</t>
+          <t>Kendall Fuller</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -864,22 +864,22 @@
         </is>
       </c>
       <c r="C17" s="3" t="n">
-        <v>1</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>10</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>8.66666666666667</v>
+        <v>45.33333333333334</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>1.33333333333333</v>
+        <v>13.33333333333333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Mike Ford</t>
+          <t>Kendall Fuller</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -888,22 +888,22 @@
         </is>
       </c>
       <c r="C18" s="3" t="n">
-        <v>0.666666666666667</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>18.6666666666667</v>
+        <v>60.33333333333334</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>13.3333333333333</v>
+        <v>42.66666666666666</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>5.33333333333333</v>
+        <v>17.66666666666667</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Mike Ford</t>
+          <t>Kendall Fuller</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -912,22 +912,22 @@
         </is>
       </c>
       <c r="C19" s="3" t="n">
-        <v>-0.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>8.66666666666667</v>
+        <v>1.666666666666671</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>4.66666666666667</v>
+        <v>-2.666666666666671</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>4</v>
+        <v>4.333333333333334</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Rock Ya-Sin</t>
+          <t>Kevin Byard</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
@@ -936,22 +936,22 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>6.666666666666667</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>46</v>
+        <v>94.33333333333333</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>39</v>
+        <v>65.33333333333333</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Rock Ya-Sin</t>
+          <t>Kevin Byard</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -960,22 +960,22 @@
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>3.666666666666667</v>
+        <v>5</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>20.33333333333333</v>
+        <v>106.4444444444444</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>16.33333333333333</v>
+        <v>67.44444444444444</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Rock Ya-Sin</t>
+          <t>Kevin Byard</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -984,22 +984,22 @@
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>-3</v>
+        <v>-4.666666666666666</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>-25.66666666666667</v>
+        <v>12.11111111111111</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>-22.66666666666667</v>
+        <v>2.111111111111114</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>D.J. Reed</t>
+          <t>Michael Davis</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1008,22 +1008,22 @@
         </is>
       </c>
       <c r="C23" s="3" t="n">
-        <v>6.333333333333333</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>51</v>
+        <v>52.33333333333334</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>39.66666666666666</v>
+        <v>40.33333333333334</v>
       </c>
       <c r="F23" s="3" t="n">
-        <v>11.33333333333333</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>D.J. Reed</t>
+          <t>Michael Davis</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1032,22 +1032,22 @@
         </is>
       </c>
       <c r="C24" s="3" t="n">
-        <v>10.66666666666667</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>73.33333333333333</v>
+        <v>46</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>59</v>
+        <v>35.66666666666666</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>14.33333333333333</v>
+        <v>10.33333333333333</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>D.J. Reed</t>
+          <t>Michael Davis</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1056,22 +1056,22 @@
         </is>
       </c>
       <c r="C25" s="3" t="n">
-        <v>4.333333333333333</v>
+        <v>-3</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>22.33333333333333</v>
+        <v>-6.333333333333336</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>19.33333333333334</v>
+        <v>-4.666666666666671</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>3</v>
+        <v>-1.666666666666666</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>Kevin Byard</t>
+          <t>Mike Ford</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
@@ -1080,22 +1080,22 @@
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>9.666666666666666</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>94.33333333333333</v>
+        <v>10</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>65.33333333333333</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>29</v>
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>Kevin Byard</t>
+          <t>Mike Ford</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
@@ -1104,22 +1104,22 @@
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>106.4444444444444</v>
+        <v>18.66666666666667</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>67.44444444444444</v>
+        <v>13.33333333333333</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>39</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>Kevin Byard</t>
+          <t>Mike Ford</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
@@ -1128,22 +1128,22 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>-4.666666666666666</v>
+        <v>-0.3333333333333334</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>12.11111111111111</v>
+        <v>8.666666666666668</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>2.111111111111114</v>
+        <v>4.666666666666668</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Michael Davis</t>
+          <t>Rock Ya-Sin</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1152,22 +1152,22 @@
         </is>
       </c>
       <c r="C29" s="3" t="n">
-        <v>11.66666666666667</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>52.33333333333334</v>
+        <v>46</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>40.33333333333334</v>
+        <v>39</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Michael Davis</t>
+          <t>Rock Ya-Sin</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1176,22 +1176,22 @@
         </is>
       </c>
       <c r="C30" s="3" t="n">
-        <v>8.666666666666666</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>46</v>
+        <v>20.33333333333333</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>35.66666666666666</v>
+        <v>16.33333333333333</v>
       </c>
       <c r="F30" s="3" t="n">
-        <v>10.33333333333333</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Michael Davis</t>
+          <t>Rock Ya-Sin</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1203,19 +1203,19 @@
         <v>-3</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>-6.333333333333336</v>
+        <v>-25.66666666666667</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>-4.666666666666671</v>
+        <v>-22.66666666666667</v>
       </c>
       <c r="F31" s="3" t="n">
-        <v>-1.666666666666666</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>Kendall Fuller</t>
+          <t>Stephon Gilmore</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
@@ -1224,22 +1224,22 @@
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>9.666666666666666</v>
+        <v>8.333333333333334</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>58.66666666666666</v>
+        <v>35.33333333333334</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>45.33333333333334</v>
+        <v>29.66666666666667</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>13.33333333333333</v>
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>Kendall Fuller</t>
+          <t>Stephon Gilmore</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
@@ -1248,22 +1248,22 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>9.666666666666666</v>
+        <v>11</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>60.33333333333334</v>
+        <v>63.33333333333334</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>42.66666666666666</v>
+        <v>49</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>17.66666666666667</v>
+        <v>14.33333333333333</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>Kendall Fuller</t>
+          <t>Stephon Gilmore</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -1272,16 +1272,16 @@
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0</v>
+        <v>2.666666666666666</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>1.666666666666671</v>
+        <v>28</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>-2.666666666666671</v>
+        <v>19.33333333333333</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>4.333333333333334</v>
+        <v>8.666666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>